<commit_message>
Modificaciones de pipeline y modelos
</commit_message>
<xml_diff>
--- a/data/labeled_test_data.xlsx
+++ b/data/labeled_test_data.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23">
@@ -1272,7 +1272,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="85">

</xml_diff>

<commit_message>
Rerun del notebook para visualización
</commit_message>
<xml_diff>
--- a/data/labeled_test_data.xlsx
+++ b/data/labeled_test_data.xlsx
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -902,7 +902,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48">
@@ -1272,7 +1272,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="85">
@@ -1302,7 +1302,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="88">

</xml_diff>